<commit_message>
ich will nicht mehr :(
</commit_message>
<xml_diff>
--- a/402/data/Balmer/h.xlsx
+++ b/402/data/Balmer/h.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="60">
   <si>
     <t>n</t>
   </si>
@@ -180,6 +180,24 @@
   </si>
   <si>
     <t>ddlambda</t>
+  </si>
+  <si>
+    <t>gamma</t>
+  </si>
+  <si>
+    <t>dgamma</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>dg</t>
+  </si>
+  <si>
+    <t>db</t>
   </si>
 </sst>
 </file>
@@ -375,11 +393,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="238689280"/>
-        <c:axId val="238711552"/>
+        <c:axId val="160627328"/>
+        <c:axId val="247302400"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="238689280"/>
+        <c:axId val="160627328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -389,12 +407,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="238711552"/>
+        <c:crossAx val="247302400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="238711552"/>
+        <c:axId val="247302400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -405,7 +423,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="238689280"/>
+        <c:crossAx val="160627328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -558,11 +576,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="220481408"/>
-        <c:axId val="220482944"/>
+        <c:axId val="141171712"/>
+        <c:axId val="141193984"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="220481408"/>
+        <c:axId val="141171712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -572,12 +590,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="220482944"/>
+        <c:crossAx val="141193984"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="220482944"/>
+        <c:axId val="141193984"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -588,7 +606,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="220481408"/>
+        <c:crossAx val="141171712"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -741,11 +759,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="220619520"/>
-        <c:axId val="220621056"/>
+        <c:axId val="21071744"/>
+        <c:axId val="21073280"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="220619520"/>
+        <c:axId val="21071744"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -755,12 +773,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="220621056"/>
+        <c:crossAx val="21073280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="220621056"/>
+        <c:axId val="21073280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -771,7 +789,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="220619520"/>
+        <c:crossAx val="21071744"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -924,11 +942,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="220652672"/>
-        <c:axId val="220654208"/>
+        <c:axId val="141062912"/>
+        <c:axId val="141064448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="220652672"/>
+        <c:axId val="141062912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -938,12 +956,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="220654208"/>
+        <c:crossAx val="141064448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="220654208"/>
+        <c:axId val="141064448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -954,7 +972,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="220652672"/>
+        <c:crossAx val="141062912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1003,7 +1021,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>'236_rc'!$R$4</c:f>
+              <c:f>'236_rc'!$T$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1027,12 +1045,12 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'236_rc'!$P$5:$P$24</c:f>
+              <c:f>'236_rc'!$R$5:$R$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>1.5824802304724477</c:v>
+                  <c:v>1.3778940589006039</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>1.1893666385365664</c:v>
@@ -1051,24 +1069,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'236_rc'!$R$5:$R$24</c:f>
+              <c:f>'236_rc'!$T$5:$T$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="20"/>
                 <c:pt idx="0">
-                  <c:v>782.74838979974186</c:v>
+                  <c:v>650.51409829174872</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>527.37354509276281</c:v>
+                  <c:v>527.38759416167738</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>447.40113249320461</c:v>
+                  <c:v>446.98738730395405</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>438.24241357429787</c:v>
+                  <c:v>437.77967589828472</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>401.09405515898959</c:v>
+                  <c:v>400.43260077663047</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1083,11 +1101,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="220593536"/>
-        <c:axId val="220677248"/>
+        <c:axId val="141122944"/>
+        <c:axId val="141132928"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="220593536"/>
+        <c:axId val="141122944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1097,12 +1115,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="220677248"/>
+        <c:crossAx val="141132928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="220677248"/>
+        <c:axId val="141132928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1113,7 +1131,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="220593536"/>
+        <c:crossAx val="141122944"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1284,13 +1302,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
+      <xdr:col>23</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>25</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>27</xdr:col>
+      <xdr:col>29</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
@@ -4836,10 +4854,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C4:W24"/>
+  <dimension ref="C1:Y24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="X5" sqref="X5:Y5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4847,7 +4865,35 @@
     <col min="6" max="6" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>56</v>
+      </c>
+      <c r="G1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" t="s">
+        <v>57</v>
+      </c>
+      <c r="I1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="3:25" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>653.096</v>
+      </c>
+      <c r="G2">
+        <v>36.47</v>
+      </c>
+      <c r="H2">
+        <v>-249.38300000000001</v>
+      </c>
+      <c r="I2">
+        <v>43.15</v>
+      </c>
+    </row>
+    <row r="4" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>0</v>
       </c>
@@ -4864,55 +4910,61 @@
         <v>40</v>
       </c>
       <c r="H4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" t="s">
         <v>47</v>
       </c>
-      <c r="I4" t="s">
+      <c r="K4" t="s">
         <v>48</v>
       </c>
-      <c r="J4" t="s">
+      <c r="L4" t="s">
         <v>41</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>42</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>49</v>
       </c>
-      <c r="M4" t="s">
+      <c r="O4" t="s">
         <v>50</v>
       </c>
-      <c r="N4" t="s">
+      <c r="P4" t="s">
         <v>43</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
         <v>44</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>1</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="S4" t="s">
         <v>2</v>
       </c>
-      <c r="R4" t="s">
+      <c r="T4" t="s">
         <v>3</v>
       </c>
-      <c r="S4" t="s">
+      <c r="U4" t="s">
         <v>4</v>
       </c>
-      <c r="T4" t="s">
+      <c r="V4" t="s">
         <v>51</v>
       </c>
-      <c r="U4" t="s">
+      <c r="W4" t="s">
         <v>52</v>
       </c>
-      <c r="V4" t="s">
+      <c r="X4" t="s">
         <v>38</v>
       </c>
-      <c r="W4" t="s">
+      <c r="Y4" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="3:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C5">
         <v>1</v>
       </c>
@@ -4923,77 +4975,85 @@
         <v>0.05</v>
       </c>
       <c r="F5">
-        <v>70</v>
+        <v>60.5</v>
       </c>
       <c r="G5">
         <v>0.5</v>
       </c>
       <c r="H5">
+        <f>D5/300</f>
+        <v>3.3333333333333338E-4</v>
+      </c>
+      <c r="I5">
+        <f>H5*SQRT((E5/D5)^2+(1/30)^2)</f>
+        <v>1.6703662642636569E-4</v>
+      </c>
+      <c r="J5">
         <f>F5*PI()/180</f>
-        <v>1.2217304763960306</v>
-      </c>
-      <c r="I5">
+        <v>1.0559241974565694</v>
+      </c>
+      <c r="K5">
         <f>G5*PI()/180</f>
         <v>8.7266462599716477E-3</v>
       </c>
-      <c r="J5">
+      <c r="L5">
         <f>(F5-30)*PI()/180</f>
-        <v>0.69813170079773179</v>
-      </c>
-      <c r="K5">
+        <v>0.53232542185827048</v>
+      </c>
+      <c r="M5">
         <f>SQRT(2)*G5*PI()/180</f>
         <v>1.2341341494884351E-2</v>
       </c>
-      <c r="L5">
-        <f t="shared" ref="L5:L9" si="0">SIN(H5)</f>
-        <v>0.93969262078590832</v>
-      </c>
-      <c r="M5">
-        <f t="shared" ref="M5:M9" si="1">COS(H5)*I5</f>
-        <v>2.9846888045879146E-3</v>
-      </c>
       <c r="N5">
-        <f>SIN(J5)</f>
-        <v>0.64278760968653925</v>
+        <f t="shared" ref="N5:N9" si="0">SIN(J5)</f>
+        <v>0.8703556959398997</v>
       </c>
       <c r="O5">
-        <f>COS(J5)*G5</f>
-        <v>0.38302222155948901</v>
-      </c>
-      <c r="P5" s="3">
-        <f>N5+L5</f>
-        <v>1.5824802304724477</v>
-      </c>
-      <c r="Q5" s="3">
-        <f>SQRT(O5*O5+M5^2)</f>
-        <v>0.38303385043051547</v>
+        <f t="shared" ref="O5:O9" si="1">COS(J5)*K5</f>
+        <v>4.2972062190988454E-3</v>
+      </c>
+      <c r="P5">
+        <f>SIN(L5)</f>
+        <v>0.50753836296070409</v>
+      </c>
+      <c r="Q5">
+        <f>COS(L5)*M5</f>
+        <v>1.0633659710959368E-2</v>
       </c>
       <c r="R5" s="3">
-        <f>649.621*P5-245.264</f>
-        <v>782.74838979974186</v>
+        <f>P5+N5</f>
+        <v>1.3778940589006039</v>
       </c>
       <c r="S5" s="3">
-        <f>SQRT(R5^2*((Q5/P5)^2+(36.27/649.621)^2)+42.7^2)</f>
-        <v>199.07008999583732</v>
-      </c>
-      <c r="T5">
-        <f>649.621*COS(J5)</f>
-        <v>497.63855718339363</v>
-      </c>
-      <c r="U5">
-        <f>T5*SQRT((36.27/649.621)^2+(N5*K5)^2)</f>
-        <v>28.063481181641748</v>
+        <f>SQRT(Q5*Q5+O5^2)</f>
+        <v>1.1469119414233259E-2</v>
+      </c>
+      <c r="T5" s="3">
+        <f>$F$2*R5+$H$2</f>
+        <v>650.51409829174872</v>
+      </c>
+      <c r="U5" s="3">
+        <f>SQRT(T5^2*((S5/R5)^2+($G$2/$F$2)^2)+$I$2^2)</f>
+        <v>56.663977701951261</v>
       </c>
       <c r="V5">
-        <f>T5*D5*PI()/180</f>
-        <v>0.86854313077242973</v>
+        <f>$F$2*COS(L5)</f>
+        <v>562.72655816771874</v>
       </c>
       <c r="W5">
-        <f>V5*SQRT((U5/T5)^2+(E5/F5)^2)</f>
-        <v>4.8983943423305441E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="3:23" x14ac:dyDescent="0.25">
+        <f>V5*SQRT(($G$2/$F$2)^2+(P5*M5)^2)</f>
+        <v>31.620681393486489</v>
+      </c>
+      <c r="X5">
+        <f>V5*H5</f>
+        <v>0.18757551938923961</v>
+      </c>
+      <c r="Y5">
+        <f>X5*SQRT((W5/V5)^2+(I5/H5)^2)</f>
+        <v>9.4585063457510499E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>2</v>
       </c>
@@ -5010,71 +5070,79 @@
         <v>0.5</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:H9" si="2">F6*PI()/180</f>
+        <f t="shared" ref="H6:H9" si="2">D6/300</f>
+        <v>1E-3</v>
+      </c>
+      <c r="I6">
+        <f>H6*SQRT((E6/D6)^2+(1/30)^2)</f>
+        <v>1.6996731711975952E-4</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ref="J6:J9" si="3">F6*PI()/180</f>
         <v>0.92502450355699462</v>
       </c>
-      <c r="I6">
-        <f t="shared" ref="I6:I9" si="3">G6*PI()/180</f>
+      <c r="K6">
+        <f t="shared" ref="K6:K9" si="4">G6*PI()/180</f>
         <v>8.7266462599716477E-3</v>
       </c>
-      <c r="J6">
+      <c r="L6">
         <f>(F6-30)*PI()/180</f>
         <v>0.40142572795869574</v>
       </c>
-      <c r="K6">
+      <c r="M6">
         <f>SQRT(2)*G6*PI()/180</f>
         <v>1.2341341494884351E-2</v>
       </c>
-      <c r="L6">
+      <c r="N6">
         <f t="shared" si="0"/>
         <v>0.79863551004729283</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <f t="shared" si="1"/>
         <v>5.251826820984574E-3</v>
       </c>
-      <c r="N6">
-        <f>SIN(J6)</f>
+      <c r="P6">
+        <f>SIN(L6)</f>
         <v>0.39073112848927372</v>
       </c>
-      <c r="O6">
-        <f>COS(J6)*G6</f>
-        <v>0.46025242672622019</v>
-      </c>
-      <c r="P6" s="3">
-        <f t="shared" ref="P6:P9" si="4">N6+L6</f>
+      <c r="Q6">
+        <f t="shared" ref="Q6:Q9" si="5">COS(L6)*M6</f>
+        <v>1.1360264744155042E-2</v>
+      </c>
+      <c r="R6" s="3">
+        <f t="shared" ref="R6:R9" si="6">P6+N6</f>
         <v>1.1893666385365664</v>
       </c>
-      <c r="Q6" s="3">
-        <f t="shared" ref="Q6:Q9" si="5">SQRT(O6*O6+M6^2)</f>
-        <v>0.46028238940060728</v>
-      </c>
-      <c r="R6" s="3">
-        <f t="shared" ref="R6:R9" si="6">649.621*P6-245.264</f>
-        <v>527.37354509276281</v>
-      </c>
       <c r="S6" s="3">
-        <f t="shared" ref="S6:S9" si="7">SQRT(R6^2*((Q6/P6)^2+(36.27/649.621)^2)+42.7^2)</f>
-        <v>210.58016239254675</v>
-      </c>
-      <c r="T6">
-        <f t="shared" ref="T6:T9" si="8">649.621*COS(J6)</f>
-        <v>597.97928340462772</v>
-      </c>
-      <c r="U6">
-        <f t="shared" ref="U6:U9" si="9">T6*SQRT((36.27/649.621)^2+(N6*K6)^2)</f>
-        <v>33.511002630607479</v>
+        <f t="shared" ref="S6:S9" si="7">SQRT(Q6*Q6+O6^2)</f>
+        <v>1.2515482412392458E-2</v>
+      </c>
+      <c r="T6" s="3">
+        <f t="shared" ref="T6:T9" si="8">$F$2*R6+$H$2</f>
+        <v>527.38759416167738</v>
+      </c>
+      <c r="U6" s="3">
+        <f t="shared" ref="U6:U9" si="9">SQRT(T6^2*((S6/R6)^2+($G$2/$F$2)^2)+$I$2^2)</f>
+        <v>52.536049052129556</v>
       </c>
       <c r="V6">
-        <f t="shared" ref="V6:V9" si="10">T6*D6*PI()/180</f>
-        <v>3.1310122062381121</v>
+        <f t="shared" ref="V6:V9" si="10">$F$2*COS(L6)</f>
+        <v>601.178037770375</v>
       </c>
       <c r="W6">
-        <f t="shared" ref="W6:W9" si="11">V6*SQRT((U6/T6)^2+(E6/F6)^2)</f>
-        <v>0.17548806002906109</v>
-      </c>
-    </row>
-    <row r="7" spans="3:23" x14ac:dyDescent="0.25">
+        <f t="shared" ref="W6:W9" si="11">V6*SQRT(($G$2/$F$2)^2+(P6*M6)^2)</f>
+        <v>33.695748051384868</v>
+      </c>
+      <c r="X6">
+        <f t="shared" ref="X6:X9" si="12">V6*H6</f>
+        <v>0.60117803777037504</v>
+      </c>
+      <c r="Y6">
+        <f>X6*SQRT((W6/V6)^2+(I6/H6)^2)</f>
+        <v>0.107593132544175</v>
+      </c>
+    </row>
+    <row r="7" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>3</v>
       </c>
@@ -5084,72 +5152,72 @@
       <c r="G7">
         <v>0.5</v>
       </c>
-      <c r="H7">
-        <f t="shared" si="2"/>
+      <c r="J7">
+        <f t="shared" si="3"/>
         <v>0.84648468721724979</v>
       </c>
-      <c r="I7">
-        <f t="shared" si="3"/>
+      <c r="K7">
+        <f t="shared" si="4"/>
         <v>8.7266462599716477E-3</v>
       </c>
-      <c r="J7">
+      <c r="L7">
         <f>(F7-30)*PI()/180</f>
         <v>0.32288591161895097</v>
       </c>
-      <c r="K7">
+      <c r="M7">
         <f>SQRT(2)*G7*PI()/180</f>
         <v>1.2341341494884351E-2</v>
       </c>
-      <c r="L7">
+      <c r="N7">
         <f t="shared" si="0"/>
         <v>0.74895572078900208</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <f t="shared" si="1"/>
         <v>5.7824507655440983E-3</v>
       </c>
-      <c r="N7">
-        <f>SIN(J7)</f>
+      <c r="P7">
+        <f>SIN(L7)</f>
         <v>0.31730465640509214</v>
       </c>
-      <c r="O7">
-        <f>COS(J7)*G7</f>
-        <v>0.47416182760309966</v>
-      </c>
-      <c r="P7" s="3">
-        <f t="shared" si="4"/>
-        <v>1.0662603771940942</v>
-      </c>
-      <c r="Q7" s="3">
+      <c r="Q7">
         <f t="shared" si="5"/>
-        <v>0.47419708507409397</v>
+        <v>1.1703586076576667E-2</v>
       </c>
       <c r="R7" s="3">
         <f t="shared" si="6"/>
-        <v>447.40113249320461</v>
+        <v>1.0662603771940942</v>
       </c>
       <c r="S7" s="3">
         <f t="shared" si="7"/>
-        <v>205.02989147935753</v>
-      </c>
-      <c r="T7">
+        <v>1.3054143553208717E-2</v>
+      </c>
+      <c r="T7" s="3">
         <f t="shared" si="8"/>
-        <v>616.05096121870645</v>
-      </c>
-      <c r="U7">
+        <v>446.98738730395405</v>
+      </c>
+      <c r="U7" s="3">
         <f t="shared" si="9"/>
-        <v>34.480196433790574</v>
+        <v>50.148765295571707</v>
       </c>
       <c r="V7">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>619.34638592054796</v>
       </c>
       <c r="W7">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="3:23" x14ac:dyDescent="0.25">
+        <v>34.670299265380429</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" ref="Y6:Y9" si="13">X7*SQRT((W7/V7)^2+(E7/F7)^2)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C8">
         <v>4</v>
       </c>
@@ -5159,72 +5227,72 @@
       <c r="G8">
         <v>0.5</v>
       </c>
-      <c r="H8">
-        <f t="shared" si="2"/>
+      <c r="J8">
+        <f t="shared" si="3"/>
         <v>0.83775804095727813</v>
       </c>
-      <c r="I8">
-        <f t="shared" si="3"/>
+      <c r="K8">
+        <f t="shared" si="4"/>
         <v>8.7266462599716477E-3</v>
       </c>
-      <c r="J8">
+      <c r="L8">
         <f>(F8-30)*PI()/180</f>
         <v>0.31415926535897931</v>
       </c>
-      <c r="K8">
+      <c r="M8">
         <f>SQRT(2)*G8*PI()/180</f>
         <v>1.2341341494884351E-2</v>
       </c>
-      <c r="L8">
+      <c r="N8">
         <f t="shared" si="0"/>
         <v>0.74314482547739413</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <f t="shared" si="1"/>
         <v>5.8392661034140907E-3</v>
       </c>
-      <c r="N8">
-        <f>SIN(J8)</f>
+      <c r="P8">
+        <f>SIN(L8)</f>
         <v>0.3090169943749474</v>
       </c>
-      <c r="O8">
-        <f>COS(J8)*G8</f>
-        <v>0.47552825814757677</v>
-      </c>
-      <c r="P8" s="3">
-        <f t="shared" si="4"/>
-        <v>1.0521618198523415</v>
-      </c>
-      <c r="Q8" s="3">
+      <c r="Q8">
         <f t="shared" si="5"/>
-        <v>0.47556410853374426</v>
+        <v>1.1737313248533533E-2</v>
       </c>
       <c r="R8" s="3">
         <f t="shared" si="6"/>
-        <v>438.24241357429787</v>
+        <v>1.0521618198523415</v>
       </c>
       <c r="S8" s="3">
         <f t="shared" si="7"/>
-        <v>204.10224194616603</v>
-      </c>
-      <c r="T8">
+        <v>1.310959766433286E-2</v>
+      </c>
+      <c r="T8" s="3">
         <f t="shared" si="8"/>
-        <v>617.82628517217393</v>
-      </c>
-      <c r="U8">
+        <v>437.77967589828472</v>
+      </c>
+      <c r="U8" s="3">
         <f t="shared" si="9"/>
-        <v>34.575197008094129</v>
+        <v>49.892885009993293</v>
       </c>
       <c r="V8">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>621.13120656629962</v>
       </c>
       <c r="W8">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="3:23" x14ac:dyDescent="0.25">
+        <v>34.765825047407176</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="3:25" x14ac:dyDescent="0.25">
       <c r="C9">
         <v>5</v>
       </c>
@@ -5234,170 +5302,170 @@
       <c r="G9">
         <v>0.5</v>
       </c>
-      <c r="H9">
-        <f t="shared" si="2"/>
+      <c r="J9">
+        <f t="shared" si="3"/>
         <v>0.80285145591739149</v>
       </c>
-      <c r="I9">
-        <f t="shared" si="3"/>
+      <c r="K9">
+        <f t="shared" si="4"/>
         <v>8.7266462599716477E-3</v>
       </c>
-      <c r="J9">
+      <c r="L9">
         <f>(F9-30)*PI()/180</f>
         <v>0.27925268031909273</v>
       </c>
-      <c r="K9">
+      <c r="M9">
         <f>SQRT(2)*G9*PI()/180</f>
         <v>1.2341341494884351E-2</v>
       </c>
-      <c r="L9">
+      <c r="N9">
         <f t="shared" si="0"/>
         <v>0.71933980033865108</v>
       </c>
-      <c r="M9">
+      <c r="O9">
         <f t="shared" si="1"/>
         <v>6.0620378705240089E-3</v>
       </c>
-      <c r="N9">
-        <f>SIN(J9)</f>
+      <c r="P9">
+        <f>SIN(L9)</f>
         <v>0.27563735581699916</v>
       </c>
-      <c r="O9">
-        <f>COS(J9)*G9</f>
-        <v>0.48063084796915945</v>
-      </c>
-      <c r="P9" s="3">
-        <f t="shared" si="4"/>
-        <v>0.99497715615565019</v>
-      </c>
-      <c r="Q9" s="3">
+      <c r="Q9">
         <f t="shared" si="5"/>
-        <v>0.48066907568793826</v>
+        <v>1.1863258855526479E-2</v>
       </c>
       <c r="R9" s="3">
         <f t="shared" si="6"/>
-        <v>401.09405515898959</v>
+        <v>0.99497715615565019</v>
       </c>
       <c r="S9" s="3">
         <f t="shared" si="7"/>
-        <v>199.6756037525077</v>
-      </c>
-      <c r="T9">
+        <v>1.3322357667353579E-2</v>
+      </c>
+      <c r="T9" s="3">
         <f t="shared" si="8"/>
-        <v>624.4557841771466</v>
-      </c>
-      <c r="U9">
+        <v>400.43260077663047</v>
+      </c>
+      <c r="U9" s="3">
         <f t="shared" si="9"/>
-        <v>34.929613807046422</v>
+        <v>48.894549177986036</v>
       </c>
       <c r="V9">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>627.79616857053236</v>
       </c>
       <c r="W9">
         <f t="shared" si="11"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
+        <v>35.122201346588589</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="3:25" x14ac:dyDescent="0.25">
       <c r="R10" s="3"/>
       <c r="S10" s="3"/>
-    </row>
-    <row r="11" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+    </row>
+    <row r="11" spans="3:25" x14ac:dyDescent="0.25">
       <c r="R11" s="3"/>
       <c r="S11" s="3"/>
-    </row>
-    <row r="12" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+    </row>
+    <row r="12" spans="3:25" x14ac:dyDescent="0.25">
       <c r="R12" s="3"/>
       <c r="S12" s="3"/>
-    </row>
-    <row r="13" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
+      <c r="T12" s="3"/>
+      <c r="U12" s="3"/>
+    </row>
+    <row r="13" spans="3:25" x14ac:dyDescent="0.25">
       <c r="R13" s="3"/>
       <c r="S13" s="3"/>
-    </row>
-    <row r="14" spans="3:23" x14ac:dyDescent="0.25">
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
+      <c r="T13" s="3"/>
+      <c r="U13" s="3"/>
+    </row>
+    <row r="14" spans="3:25" x14ac:dyDescent="0.25">
       <c r="R14" s="3"/>
       <c r="S14" s="3"/>
-    </row>
-    <row r="15" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+    </row>
+    <row r="15" spans="3:25" x14ac:dyDescent="0.25">
       <c r="D15" s="3"/>
-      <c r="P15" s="3"/>
-      <c r="Q15" s="3"/>
       <c r="R15" s="3"/>
       <c r="S15" s="3"/>
-    </row>
-    <row r="16" spans="3:23" x14ac:dyDescent="0.25">
+      <c r="T15" s="3"/>
+      <c r="U15" s="3"/>
+    </row>
+    <row r="16" spans="3:25" x14ac:dyDescent="0.25">
       <c r="D16" s="3"/>
-      <c r="P16" s="3"/>
-      <c r="Q16" s="3"/>
       <c r="R16" s="3"/>
       <c r="S16" s="3"/>
-    </row>
-    <row r="17" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T16" s="3"/>
+      <c r="U16" s="3"/>
+    </row>
+    <row r="17" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D17" s="3"/>
-      <c r="P17" s="3"/>
-      <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
       <c r="S17" s="3"/>
-    </row>
-    <row r="18" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T17" s="3"/>
+      <c r="U17" s="3"/>
+    </row>
+    <row r="18" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D18" s="3"/>
-      <c r="P18" s="3"/>
-      <c r="Q18" s="3"/>
       <c r="R18" s="3"/>
       <c r="S18" s="3"/>
-    </row>
-    <row r="19" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T18" s="3"/>
+      <c r="U18" s="3"/>
+    </row>
+    <row r="19" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D19" s="3"/>
-      <c r="P19" s="3"/>
-      <c r="Q19" s="3"/>
       <c r="R19" s="3"/>
       <c r="S19" s="3"/>
-    </row>
-    <row r="20" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T19" s="3"/>
+      <c r="U19" s="3"/>
+    </row>
+    <row r="20" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D20" s="3"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="3"/>
       <c r="R20" s="3"/>
       <c r="S20" s="3"/>
-    </row>
-    <row r="21" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T20" s="3"/>
+      <c r="U20" s="3"/>
+    </row>
+    <row r="21" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D21" s="3"/>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
       <c r="R21" s="3"/>
       <c r="S21" s="3"/>
-    </row>
-    <row r="22" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T21" s="3"/>
+      <c r="U21" s="3"/>
+    </row>
+    <row r="22" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D22" s="3"/>
-      <c r="P22" s="3"/>
-      <c r="Q22" s="3"/>
       <c r="R22" s="3"/>
       <c r="S22" s="3"/>
-    </row>
-    <row r="23" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T22" s="3"/>
+      <c r="U22" s="3"/>
+    </row>
+    <row r="23" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D23" s="3"/>
-      <c r="P23" s="3"/>
-      <c r="Q23" s="3"/>
       <c r="R23" s="3"/>
       <c r="S23" s="3"/>
-    </row>
-    <row r="24" spans="4:19" x14ac:dyDescent="0.25">
+      <c r="T23" s="3"/>
+      <c r="U23" s="3"/>
+    </row>
+    <row r="24" spans="4:21" x14ac:dyDescent="0.25">
       <c r="D24" s="3"/>
-      <c r="P24" s="3"/>
-      <c r="Q24" s="3"/>
       <c r="R24" s="3"/>
       <c r="S24" s="3"/>
+      <c r="T24" s="3"/>
+      <c r="U24" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>